<commit_message>
Atualizando o cronograma e melhorando a justificativa
</commit_message>
<xml_diff>
--- a/Cronogramas/CRONOGRAMA-04 - GRUPO-02.xlsx
+++ b/Cronogramas/CRONOGRAMA-04 - GRUPO-02.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOGIMIRIM-CLODOVEUBA\Documents\GitHub\TCC\Cronogramas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA82BEA-5052-46EE-888F-85942E22B852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5CAEE2-3A8E-4083-91DC-6C1683680896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,32 +481,32 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F779B1-8D3E-4391-A788-FB6D40123DAC}">
   <dimension ref="B1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -842,44 +842,44 @@
   <sheetData>
     <row r="1" spans="2:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="25.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="2:9" ht="25.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="26"/>
     </row>
     <row r="4" spans="2:9" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="23"/>
+      <c r="D4" s="27"/>
     </row>
     <row r="5" spans="2:9" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C5" s="1"/>
       <c r="G5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="25"/>
+      <c r="I5" s="29"/>
     </row>
     <row r="6" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="9" t="s">
@@ -905,7 +905,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -924,11 +924,10 @@
         <f>F7-E7</f>
         <v>14</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="6"/>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="20"/>
+      <c r="B8" s="24"/>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
@@ -943,7 +942,7 @@
       <c r="I8" s="7"/>
     </row>
     <row r="9" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="20"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="4" t="s">
         <v>2</v>
       </c>
@@ -958,7 +957,7 @@
       <c r="I9" s="7"/>
     </row>
     <row r="10" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="20"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="4" t="s">
         <v>2</v>
       </c>
@@ -973,7 +972,7 @@
       <c r="I10" s="7"/>
     </row>
     <row r="11" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="20"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="5" t="s">
         <v>2</v>
       </c>
@@ -984,11 +983,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H11" s="26"/>
+      <c r="H11" s="19"/>
       <c r="I11" s="8"/>
     </row>
     <row r="12" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="20"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1001,15 +1000,14 @@
       <c r="F12" s="3">
         <v>45433</v>
       </c>
-      <c r="G12" s="29">
+      <c r="G12" s="22">
         <f>F12-E12</f>
         <v>14</v>
       </c>
-      <c r="H12" s="28"/>
       <c r="I12" s="30"/>
     </row>
     <row r="13" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="20"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1024,7 +1022,7 @@
       <c r="I13" s="7"/>
     </row>
     <row r="14" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="20"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="4" t="s">
         <v>2</v>
       </c>
@@ -1039,7 +1037,7 @@
       <c r="I14" s="7"/>
     </row>
     <row r="15" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="20"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="4" t="s">
         <v>2</v>
       </c>
@@ -1054,7 +1052,7 @@
       <c r="I15" s="7"/>
     </row>
     <row r="16" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="20"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="5" t="s">
         <v>2</v>
       </c>
@@ -1065,11 +1063,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
     </row>
     <row r="17" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="20"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1082,15 +1080,15 @@
       <c r="F17" s="3">
         <v>45422</v>
       </c>
-      <c r="G17" s="29">
+      <c r="G17" s="22">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="28"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21"/>
     </row>
     <row r="18" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="20"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
@@ -1105,7 +1103,7 @@
       <c r="I18" s="7"/>
     </row>
     <row r="19" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="20"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="4" t="s">
         <v>2</v>
       </c>
@@ -1120,7 +1118,7 @@
       <c r="I19" s="7"/>
     </row>
     <row r="20" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="20"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="4" t="s">
         <v>2</v>
       </c>
@@ -1135,7 +1133,7 @@
       <c r="I20" s="7"/>
     </row>
     <row r="21" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="20"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="5" t="s">
         <v>2</v>
       </c>
@@ -1150,7 +1148,7 @@
       <c r="I21" s="8"/>
     </row>
     <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="20"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="3" t="s">
         <v>23</v>
       </c>
@@ -1171,7 +1169,7 @@
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="20"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="4" t="s">
         <v>2</v>
       </c>
@@ -1186,7 +1184,7 @@
       <c r="I23" s="7"/>
     </row>
     <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="20"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="4" t="s">
         <v>2</v>
       </c>
@@ -1201,7 +1199,7 @@
       <c r="I24" s="7"/>
     </row>
     <row r="25" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="20"/>
+      <c r="B25" s="24"/>
       <c r="C25" s="4" t="s">
         <v>2</v>
       </c>
@@ -1216,7 +1214,7 @@
       <c r="I25" s="7"/>
     </row>
     <row r="26" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="20"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="5" t="s">
         <v>2</v>
       </c>
@@ -1231,7 +1229,7 @@
       <c r="I26" s="8"/>
     </row>
     <row r="27" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="20"/>
+      <c r="B27" s="24"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
         <v>16</v>
@@ -1245,7 +1243,7 @@
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="20"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="4" t="s">
         <v>2</v>
       </c>
@@ -1260,7 +1258,7 @@
       <c r="I28" s="7"/>
     </row>
     <row r="29" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="20"/>
+      <c r="B29" s="24"/>
       <c r="C29" s="4" t="s">
         <v>2</v>
       </c>
@@ -1275,7 +1273,7 @@
       <c r="I29" s="7"/>
     </row>
     <row r="30" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="20"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="4" t="s">
         <v>2</v>
       </c>
@@ -1290,7 +1288,7 @@
       <c r="I30" s="7"/>
     </row>
     <row r="31" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="20"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="5" t="s">
         <v>2</v>
       </c>
@@ -1305,7 +1303,7 @@
       <c r="I31" s="8"/>
     </row>
     <row r="32" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="20"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="3" t="s">
         <v>2</v>
       </c>
@@ -1320,7 +1318,7 @@
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="20"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="4" t="s">
         <v>2</v>
       </c>
@@ -1335,7 +1333,7 @@
       <c r="I33" s="7"/>
     </row>
     <row r="34" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="20"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="4" t="s">
         <v>2</v>
       </c>
@@ -1350,7 +1348,7 @@
       <c r="I34" s="7"/>
     </row>
     <row r="35" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="20"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="4" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1363,7 @@
       <c r="I35" s="7"/>
     </row>
     <row r="36" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="20"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="5" t="s">
         <v>2</v>
       </c>

</xml_diff>